<commit_message>
Update backend: Entity, Repository, API DTO, DTO
</commit_message>
<xml_diff>
--- a/document/references-document/einvoicehub_softz/HĐĐT/Model_EInvoice.xlsx
+++ b/document/references-document/einvoicehub_softz/HĐĐT/Model_EInvoice.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865"/>
   </bookViews>
   <sheets>
     <sheet name="Phân tích tổng quát" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="570">
   <si>
     <t>Nhóm chức năng</t>
   </si>
@@ -4508,13 +4508,22 @@
   </si>
   <si>
     <t>N/A (Có API cập nhật trạng thái)</t>
+  </si>
+  <si>
+    <t>PHÂN TÍCH TỔNG QUÁT</t>
+  </si>
+  <si>
+    <t>SO SÁNH CHỨC NĂNG</t>
+  </si>
+  <si>
+    <t>SO SÁNH DỮ LIỆU ĐẦU VÀO PHÁT HÀNH HÓA ĐƠN ĐIỆN TỬ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4569,6 +4578,19 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -4602,7 +4624,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -4699,11 +4721,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4741,6 +4772,21 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4752,15 +4798,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5096,10 +5133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5109,1010 +5146,2364 @@
     <col min="3" max="3" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="20.25">
+      <c r="A1" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21.6" customHeight="1">
-      <c r="A2" s="16" t="s">
+    <row r="3" spans="1:3" ht="21.6" customHeight="1">
+      <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-    </row>
-    <row r="3" spans="1:3" ht="31.5">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:3" ht="31.5">
+      <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="4">
         <v>100</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="31.5">
-      <c r="A4" s="14"/>
-      <c r="B4" s="4">
+    <row r="5" spans="1:3" ht="31.5">
+      <c r="A5" s="19"/>
+      <c r="B5" s="4">
         <v>101</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5">
-      <c r="A5" s="14"/>
-      <c r="B5" s="4">
+    <row r="6" spans="1:3" ht="31.5">
+      <c r="A6" s="19"/>
+      <c r="B6" s="4">
         <v>110</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5">
-      <c r="A6" s="14"/>
-      <c r="B6" s="4">
+    <row r="7" spans="1:3" ht="31.5">
+      <c r="A7" s="19"/>
+      <c r="B7" s="4">
         <v>111</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5">
-      <c r="A7" s="14"/>
-      <c r="B7" s="4">
+    <row r="8" spans="1:3" ht="31.5">
+      <c r="A8" s="19"/>
+      <c r="B8" s="4">
         <v>112</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="1:3" ht="31.5">
+      <c r="A9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5">
-      <c r="A9" s="14"/>
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:3" ht="31.5">
+      <c r="A10" s="19"/>
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5">
-      <c r="A10" s="14"/>
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:3" ht="31.5">
+      <c r="A11" s="19"/>
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5">
-      <c r="A11" s="14"/>
-      <c r="B11" s="4" t="s">
+    <row r="12" spans="1:3" ht="31.5">
+      <c r="A12" s="19"/>
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5">
-      <c r="A12" s="14"/>
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:3" ht="31.5">
+      <c r="A13" s="19"/>
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="14"/>
-      <c r="B13" s="4" t="s">
+    <row r="14" spans="1:3" ht="15.75">
+      <c r="A14" s="19"/>
+      <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="31.5">
-      <c r="A14" s="14"/>
-      <c r="B14" s="4" t="s">
+    <row r="15" spans="1:3" ht="31.5">
+      <c r="A15" s="19"/>
+      <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5">
-      <c r="A15" s="15"/>
-      <c r="B15" s="4">
+    <row r="16" spans="1:3" ht="31.5">
+      <c r="A16" s="20"/>
+      <c r="B16" s="4">
         <v>300</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.5">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:3" ht="31.5">
+      <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5">
-      <c r="A17" s="13" t="s">
+    <row r="18" spans="1:3" ht="31.5">
+      <c r="A18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B18" s="4">
         <v>800</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="31.5">
-      <c r="A18" s="14"/>
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="1:3" ht="31.5">
+      <c r="A19" s="19"/>
+      <c r="B19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75">
-      <c r="A19" s="14"/>
-      <c r="B19" s="4">
+    <row r="20" spans="1:3" ht="15.75">
+      <c r="A20" s="19"/>
+      <c r="B20" s="4">
         <v>802</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.5">
-      <c r="A20" s="14"/>
-      <c r="B20" s="4" t="s">
+    <row r="21" spans="1:3" ht="31.5">
+      <c r="A21" s="19"/>
+      <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75">
-      <c r="A21" s="14"/>
-      <c r="B21" s="4" t="s">
+    <row r="22" spans="1:3" ht="15.75">
+      <c r="A22" s="19"/>
+      <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5">
-      <c r="A22" s="14"/>
-      <c r="B22" s="4">
+    <row r="23" spans="1:3" ht="31.5">
+      <c r="A23" s="19"/>
+      <c r="B23" s="4">
         <v>810</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5">
-      <c r="A23" s="14"/>
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="1:3" ht="31.5">
+      <c r="A24" s="19"/>
+      <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5">
-      <c r="A24" s="15"/>
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="1:3" ht="31.5">
+      <c r="A25" s="20"/>
+      <c r="B25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.5">
-      <c r="A25" s="13" t="s">
+    <row r="26" spans="1:3" ht="31.5">
+      <c r="A26" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="1:3" ht="24" customHeight="1">
+      <c r="A27" s="19"/>
+      <c r="B27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="23.45" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="4">
+    <row r="28" spans="1:3" ht="23.45" customHeight="1">
+      <c r="A28" s="20"/>
+      <c r="B28" s="4">
         <v>904</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="19.149999999999999" customHeight="1">
-      <c r="A28" s="16" t="s">
+    <row r="29" spans="1:3" ht="19.149999999999999" customHeight="1">
+      <c r="A29" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75">
-      <c r="A29" s="13" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75">
+      <c r="A30" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75">
-      <c r="A30" s="14"/>
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="1:3" ht="15.75">
+      <c r="A31" s="19"/>
+      <c r="B31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="31.5">
-      <c r="A31" s="15"/>
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:3" ht="31.5">
+      <c r="A32" s="20"/>
+      <c r="B32" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75">
-      <c r="A32" s="13" t="s">
+    <row r="33" spans="1:3" ht="15.75">
+      <c r="A33" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.5">
-      <c r="A33" s="15"/>
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="1:3" ht="31.5">
+      <c r="A34" s="20"/>
+      <c r="B34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75">
-      <c r="A34" s="13" t="s">
+    <row r="35" spans="1:3" ht="15.75">
+      <c r="A35" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:3" ht="47.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="20.45" customHeight="1">
-      <c r="A36" s="13" t="s">
+    <row r="37" spans="1:3" ht="20.45" customHeight="1">
+      <c r="A37" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="19.149999999999999" customHeight="1">
-      <c r="A37" s="14"/>
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:3" ht="19.149999999999999" customHeight="1">
+      <c r="A38" s="19"/>
+      <c r="B38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" customHeight="1">
-      <c r="A38" s="15"/>
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:3" ht="21" customHeight="1">
+      <c r="A39" s="20"/>
+      <c r="B39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="19.149999999999999" customHeight="1">
-      <c r="A39" s="16" t="s">
+    <row r="40" spans="1:3" ht="19.149999999999999" customHeight="1">
+      <c r="A40" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-    </row>
-    <row r="40" spans="1:3" ht="31.5">
-      <c r="A40" s="13" t="s">
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+    </row>
+    <row r="41" spans="1:3" ht="31.5">
+      <c r="A41" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="47.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="4" t="s">
+    <row r="42" spans="1:3" ht="47.25">
+      <c r="A42" s="19"/>
+      <c r="B42" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="47.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="4" t="s">
+    <row r="43" spans="1:3" ht="47.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5">
-      <c r="A43" s="14"/>
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:3" ht="31.5">
+      <c r="A44" s="19"/>
+      <c r="B44" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="31.5">
-      <c r="A44" s="14"/>
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:3" ht="31.5">
+      <c r="A45" s="19"/>
+      <c r="B45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="31.5">
-      <c r="A45" s="14"/>
-      <c r="B45" s="4" t="s">
+    <row r="46" spans="1:3" ht="31.5">
+      <c r="A46" s="19"/>
+      <c r="B46" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75">
-      <c r="A46" s="15"/>
-      <c r="B46" s="4" t="s">
+    <row r="47" spans="1:3" ht="15.75">
+      <c r="A47" s="20"/>
+      <c r="B47" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75">
-      <c r="A47" s="13" t="s">
+    <row r="48" spans="1:3" ht="15.75">
+      <c r="A48" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="31.5">
-      <c r="A48" s="15"/>
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:3" ht="31.5">
+      <c r="A49" s="20"/>
+      <c r="B49" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75">
-      <c r="A49" s="13" t="s">
+    <row r="50" spans="1:3" ht="15.75">
+      <c r="A50" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75">
-      <c r="A50" s="14"/>
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:3" ht="15.75">
+      <c r="A51" s="19"/>
+      <c r="B51" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75">
-      <c r="A51" s="14"/>
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:3" ht="15.75">
+      <c r="A52" s="19"/>
+      <c r="B52" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75">
-      <c r="A52" s="14"/>
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:3" ht="15.75">
+      <c r="A53" s="19"/>
+      <c r="B53" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75">
-      <c r="A53" s="14"/>
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:3" ht="15.75">
+      <c r="A54" s="19"/>
+      <c r="B54" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="31.5">
-      <c r="A54" s="14"/>
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:3" ht="31.5">
+      <c r="A55" s="19"/>
+      <c r="B55" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="31.5">
-      <c r="A55" s="14"/>
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:3" ht="31.5">
+      <c r="A56" s="19"/>
+      <c r="B56" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75">
-      <c r="A56" s="14"/>
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:3" ht="15.75">
+      <c r="A57" s="19"/>
+      <c r="B57" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="31.5">
-      <c r="A57" s="14"/>
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:3" ht="31.5">
+      <c r="A58" s="19"/>
+      <c r="B58" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="31.5">
-      <c r="A58" s="15"/>
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:3" ht="31.5">
+      <c r="A59" s="20"/>
+      <c r="B59" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75">
-      <c r="A59" s="13" t="s">
+    <row r="60" spans="1:3" ht="15.75">
+      <c r="A60" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75">
-      <c r="A60" s="14"/>
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:3" ht="15.75">
+      <c r="A61" s="19"/>
+      <c r="B61" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75">
-      <c r="A61" s="15"/>
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:3" ht="15.75">
+      <c r="A62" s="20"/>
+      <c r="B62" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="20.45" customHeight="1">
-      <c r="A62" s="16" t="s">
+    <row r="63" spans="1:3" ht="20.45" customHeight="1">
+      <c r="A63" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-    </row>
-    <row r="63" spans="1:3" ht="15.75">
-      <c r="A63" s="13" t="s">
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.75">
+      <c r="A64" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B64" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="31.5">
-      <c r="A64" s="14"/>
-      <c r="B64" s="8" t="s">
+    <row r="65" spans="1:3" ht="31.5">
+      <c r="A65" s="19"/>
+      <c r="B65" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75">
-      <c r="A65" s="14"/>
-      <c r="B65" s="8" t="s">
+    <row r="66" spans="1:3" ht="15.75">
+      <c r="A66" s="19"/>
+      <c r="B66" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75">
-      <c r="A66" s="14"/>
-      <c r="B66" s="8" t="s">
+    <row r="67" spans="1:3" ht="15.75">
+      <c r="A67" s="19"/>
+      <c r="B67" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C67" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="31.5">
-      <c r="A67" s="15"/>
-      <c r="B67" s="8" t="s">
+    <row r="68" spans="1:3" ht="31.5">
+      <c r="A68" s="20"/>
+      <c r="B68" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C68" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75">
-      <c r="A68" s="13" t="s">
+    <row r="69" spans="1:3" ht="15.75">
+      <c r="A69" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B69" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75">
-      <c r="A69" s="15"/>
-      <c r="B69" s="8" t="s">
+    <row r="70" spans="1:3" ht="15.75">
+      <c r="A70" s="20"/>
+      <c r="B70" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75">
-      <c r="A70" s="13" t="s">
+    <row r="71" spans="1:3" ht="15.75">
+      <c r="A71" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B71" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C71" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="31.5">
-      <c r="A71" s="15"/>
-      <c r="B71" s="8" t="s">
+    <row r="72" spans="1:3" ht="31.5">
+      <c r="A72" s="20"/>
+      <c r="B72" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="31.5">
-      <c r="A72" s="13" t="s">
+    <row r="73" spans="1:3" ht="31.5">
+      <c r="A73" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B73" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C73" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="31.5">
-      <c r="A73" s="14"/>
-      <c r="B73" s="8" t="s">
+    <row r="74" spans="1:3" ht="31.5">
+      <c r="A74" s="19"/>
+      <c r="B74" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C74" s="6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="31.5">
-      <c r="A74" s="14"/>
-      <c r="B74" s="8" t="s">
+    <row r="75" spans="1:3" ht="31.5">
+      <c r="A75" s="19"/>
+      <c r="B75" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C75" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75">
-      <c r="A75" s="15"/>
-      <c r="B75" s="8" t="s">
+    <row r="76" spans="1:3" ht="15.75">
+      <c r="A76" s="20"/>
+      <c r="B76" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C76" s="6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75">
-      <c r="A76" s="4" t="s">
+    <row r="77" spans="1:3" ht="15.75">
+      <c r="A77" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B77" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C77" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75">
-      <c r="A77" s="13" t="s">
+    <row r="78" spans="1:3" ht="31.5">
+      <c r="A78" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B78" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="31.5">
-      <c r="A78" s="14"/>
-      <c r="B78" s="8" t="s">
+    <row r="79" spans="1:3" ht="31.5">
+      <c r="A79" s="19"/>
+      <c r="B79" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75">
-      <c r="A79" s="14"/>
-      <c r="B79" s="8" t="s">
+    <row r="80" spans="1:3" ht="15.75">
+      <c r="A80" s="19"/>
+      <c r="B80" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C80" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="31.5">
-      <c r="A80" s="15"/>
-      <c r="B80" s="8" t="s">
+    <row r="81" spans="1:3" ht="31.5">
+      <c r="A81" s="20"/>
+      <c r="B81" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C81" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="31.5">
-      <c r="A81" s="13" t="s">
+    <row r="82" spans="1:3" ht="31.5">
+      <c r="A82" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B82" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C82" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75">
-      <c r="A82" s="15"/>
-      <c r="B82" s="8" t="s">
+    <row r="83" spans="1:3" ht="15.75">
+      <c r="A83" s="20"/>
+      <c r="B83" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C83" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.75">
-      <c r="A83" s="13" t="s">
+    <row r="84" spans="1:3" ht="15.75">
+      <c r="A84" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B84" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C84" s="6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="31.5">
-      <c r="A84" s="14"/>
-      <c r="B84" s="8" t="s">
+    <row r="85" spans="1:3" ht="31.5">
+      <c r="A85" s="19"/>
+      <c r="B85" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75">
-      <c r="A85" s="15"/>
-      <c r="B85" s="8" t="s">
+    <row r="86" spans="1:3" ht="15.75">
+      <c r="A86" s="20"/>
+      <c r="B86" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C86" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="31.5">
-      <c r="A86" s="13" t="s">
+    <row r="87" spans="1:3" ht="31.5">
+      <c r="A87" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B87" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="31.5">
-      <c r="A87" s="15"/>
-      <c r="B87" s="8" t="s">
+    <row r="88" spans="1:3" ht="31.5">
+      <c r="A88" s="20"/>
+      <c r="B88" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C88" s="6" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="31.5">
-      <c r="A88" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="31.5">
       <c r="A89" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="31.5">
+      <c r="A90" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B90" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C90" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75">
-      <c r="A90" s="4" t="s">
+    <row r="91" spans="1:3" ht="15.75">
+      <c r="A91" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B91" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C91" s="6" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="31.5">
-      <c r="A91" s="13" t="s">
+    <row r="92" spans="1:3" ht="31.5">
+      <c r="A92" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B92" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="31.5">
-      <c r="A92" s="15"/>
-      <c r="B92" s="8" t="s">
+    <row r="93" spans="1:3" ht="31.5">
+      <c r="A93" s="20"/>
+      <c r="B93" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="21.6" customHeight="1">
-      <c r="A93" s="13" t="s">
+    <row r="94" spans="1:3" ht="21.6" customHeight="1">
+      <c r="A94" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B94" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C94" s="6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="24" customHeight="1">
-      <c r="A94" s="14"/>
-      <c r="B94" s="8" t="s">
+    <row r="95" spans="1:3" ht="24" customHeight="1">
+      <c r="A95" s="19"/>
+      <c r="B95" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C95" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="31.5">
-      <c r="A95" s="15"/>
-      <c r="B95" s="8" t="s">
+    <row r="96" spans="1:3" ht="31.5">
+      <c r="A96" s="20"/>
+      <c r="B96" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="C96" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="19.149999999999999" customHeight="1">
-      <c r="A96" s="13" t="s">
+    <row r="97" spans="1:6" ht="19.149999999999999" customHeight="1">
+      <c r="A97" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B97" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C97" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="21" customHeight="1">
-      <c r="A97" s="14"/>
-      <c r="B97" s="8" t="s">
+    <row r="98" spans="1:6" ht="21" customHeight="1">
+      <c r="A98" s="19"/>
+      <c r="B98" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="31.5">
-      <c r="A98" s="15"/>
-      <c r="B98" s="8" t="s">
+    <row r="99" spans="1:6" ht="31.5">
+      <c r="A99" s="20"/>
+      <c r="B99" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="31.5">
-      <c r="A99" s="4" t="s">
+    <row r="100" spans="1:6" ht="31.5">
+      <c r="A100" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B99" s="8" t="s">
+      <c r="B100" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="C100" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="47.25">
-      <c r="A100" s="4" t="s">
+    <row r="101" spans="1:6" ht="47.25">
+      <c r="A101" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B101" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C101" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="31.5">
-      <c r="A101" s="13" t="s">
+    <row r="102" spans="1:6" ht="31.5">
+      <c r="A102" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="B102" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C102" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="31.5">
-      <c r="A102" s="15"/>
-      <c r="B102" s="8" t="s">
+    <row r="103" spans="1:6" ht="31.5">
+      <c r="A103" s="20"/>
+      <c r="B103" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C103" s="6" t="s">
         <v>215</v>
       </c>
     </row>
+    <row r="106" spans="1:6" ht="20.25">
+      <c r="A106" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="B106" s="16"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="16"/>
+      <c r="E106" s="16"/>
+      <c r="F106" s="16"/>
+    </row>
+    <row r="107" spans="1:6" ht="93.75">
+      <c r="A107" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="47.25">
+      <c r="A108" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="78.75">
+      <c r="A109" s="19"/>
+      <c r="B109" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="47.25">
+      <c r="A110" s="19"/>
+      <c r="B110" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="78.75">
+      <c r="A111" s="19"/>
+      <c r="B111" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="78.75">
+      <c r="A112" s="20"/>
+      <c r="B112" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="94.5">
+      <c r="A113" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="94.5">
+      <c r="A114" s="19"/>
+      <c r="B114" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="47.25">
+      <c r="A115" s="19"/>
+      <c r="B115" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="63">
+      <c r="A116" s="20"/>
+      <c r="B116" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="63">
+      <c r="A117" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="63">
+      <c r="A118" s="19"/>
+      <c r="B118" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="78.75">
+      <c r="A119" s="19"/>
+      <c r="B119" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="63">
+      <c r="A120" s="19"/>
+      <c r="B120" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="78.75">
+      <c r="A121" s="20"/>
+      <c r="B121" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:6" ht="63">
+      <c r="A122" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="63">
+      <c r="A123" s="19"/>
+      <c r="B123" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="110.25">
+      <c r="A124" s="19"/>
+      <c r="B124" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="47.25">
+      <c r="A125" s="19"/>
+      <c r="B125" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="63">
+      <c r="A126" s="19"/>
+      <c r="B126" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="63">
+      <c r="A127" s="20"/>
+      <c r="B127" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="63">
+      <c r="A128" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F128" s="5"/>
+    </row>
+    <row r="129" spans="1:6" ht="78.75">
+      <c r="A129" s="19"/>
+      <c r="B129" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="78.75">
+      <c r="A130" s="20"/>
+      <c r="B130" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="78.75">
+      <c r="A131" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="63">
+      <c r="A132" s="19"/>
+      <c r="B132" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" ht="47.25">
+      <c r="A133" s="19"/>
+      <c r="B133" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="15.75">
+      <c r="A134" s="19"/>
+      <c r="B134" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" ht="78.75">
+      <c r="A135" s="19"/>
+      <c r="B135" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="47.25">
+      <c r="A136" s="19"/>
+      <c r="B136" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6" ht="94.5">
+      <c r="A137" s="19"/>
+      <c r="B137" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="63">
+      <c r="A138" s="20"/>
+      <c r="B138" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="20.25">
+      <c r="A141" s="16" t="s">
+        <v>569</v>
+      </c>
+      <c r="B141" s="16"/>
+      <c r="C141" s="16"/>
+      <c r="D141" s="16"/>
+      <c r="E141" s="16"/>
+      <c r="F141" s="16"/>
+    </row>
+    <row r="142" spans="1:6" ht="63">
+      <c r="A142" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D142" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="E142" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="F142" s="12" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="15.75">
+      <c r="A143" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B143" s="14"/>
+      <c r="C143" s="14"/>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
+      <c r="F143" s="15"/>
+    </row>
+    <row r="144" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A144" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D144" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="E144" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="F144" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="63">
+      <c r="A145" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="D145" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E145" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="F145" s="7" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="78.75">
+      <c r="A146" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="D146" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="15.75">
+      <c r="A147" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="B147" s="14"/>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+      <c r="F147" s="15"/>
+    </row>
+    <row r="148" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A148" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D148" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="F148" s="7" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="63">
+      <c r="A149" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D149" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="F149" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="110.25">
+      <c r="A150" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D150" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="F150" s="11" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="78.75">
+      <c r="A151" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C151" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="63">
+      <c r="A152" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C152" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="D152" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="E152" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="F152" s="11" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="94.5">
+      <c r="A153" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C153" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="E153" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="F153" s="11" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="94.5">
+      <c r="A154" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C154" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="D154" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="E154" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="F154" s="7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="15.75">
+      <c r="A155" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="B155" s="14"/>
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
+      <c r="F155" s="15"/>
+    </row>
+    <row r="156" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A156" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="D156" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="E156" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="F156" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="47.25">
+      <c r="A157" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="D157" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="F157" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="47.25">
+      <c r="A158" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C158" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="D158" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="E158" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="F158" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="63">
+      <c r="A159" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="D159" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="E159" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="F159" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="47.25">
+      <c r="A160" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="D160" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="E160" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="F160" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="15.75">
+      <c r="A161" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="B161" s="14"/>
+      <c r="C161" s="14"/>
+      <c r="D161" s="14"/>
+      <c r="E161" s="14"/>
+      <c r="F161" s="15"/>
+    </row>
+    <row r="162" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A162" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C162" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="E162" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="F162" s="11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="47.25">
+      <c r="A163" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C163" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="D163" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="E163" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F163" s="11" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="78.75">
+      <c r="A164" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C164" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="D164" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="E164" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="F164" s="11" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="78.75">
+      <c r="A165" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C165" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="D165" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="F165" s="11" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="78.75">
+      <c r="A166" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C166" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="D166" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="F166" s="11" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="78.75">
+      <c r="A167" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C167" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="D167" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="E167" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="F167" s="11" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="47.25">
+      <c r="A168" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C168" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="D168" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="E168" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="F168" s="11" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="31.5">
+      <c r="A169" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="E169" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="78.75">
+      <c r="A170" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="E170" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="F170" s="7" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="63">
+      <c r="A171" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E171" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="F171" s="7" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="15.75">
+      <c r="A172" s="13" t="s">
+        <v>514</v>
+      </c>
+      <c r="B172" s="14"/>
+      <c r="C172" s="14"/>
+      <c r="D172" s="14"/>
+      <c r="E172" s="14"/>
+      <c r="F172" s="15"/>
+    </row>
+    <row r="173" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A173" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="D173" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="E173" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="F173" s="11" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="47.25">
+      <c r="A174" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="D174" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="E174" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="F174" s="7" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="63">
+      <c r="A175" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="C175" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="D175" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="E175" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="78.75">
+      <c r="A176" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="D176" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="E176" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="F176" s="7" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="63">
+      <c r="A177" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="D177" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="E177" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="F177" s="11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="15.75">
+      <c r="A178" s="13" t="s">
+        <v>545</v>
+      </c>
+      <c r="B178" s="14"/>
+      <c r="C178" s="14"/>
+      <c r="D178" s="14"/>
+      <c r="E178" s="14"/>
+      <c r="F178" s="15"/>
+    </row>
+    <row r="179" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A179" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="D179" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="E179" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="F179" s="7" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="94.5">
+      <c r="A180" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="D180" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="E180" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="F180" s="7" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="94.5">
+      <c r="A181" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E181" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="F181" s="7" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="63">
+      <c r="A182" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C182" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D182" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="E182" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="F182" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A17:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A93:A95"/>
+  <mergeCells count="43">
+    <mergeCell ref="A106:F106"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A108:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A117:A121"/>
+    <mergeCell ref="A122:A127"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="A131:A138"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A161:F161"/>
+    <mergeCell ref="A172:F172"/>
+    <mergeCell ref="A178:F178"/>
+    <mergeCell ref="A141:F141"/>
+    <mergeCell ref="A147:F147"/>
+    <mergeCell ref="A143:F143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6123,8 +7514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F32"/>
+    <sheetView topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6158,7 +7549,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.15" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="18" t="s">
         <v>222</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -6178,7 +7569,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="57.6" customHeight="1">
-      <c r="A3" s="14"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>228</v>
       </c>
@@ -6196,7 +7587,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="69" customHeight="1">
-      <c r="A4" s="14"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>233</v>
       </c>
@@ -6214,7 +7605,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="45.6" customHeight="1">
-      <c r="A5" s="14"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="4" t="s">
         <v>238</v>
       </c>
@@ -6232,7 +7623,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="67.150000000000006" customHeight="1">
-      <c r="A6" s="15"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>242</v>
       </c>
@@ -6250,7 +7641,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="85.15" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="18" t="s">
         <v>247</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -6268,7 +7659,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="66.599999999999994" customHeight="1">
-      <c r="A8" s="14"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>252</v>
       </c>
@@ -6284,7 +7675,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="42.6" customHeight="1">
-      <c r="A9" s="14"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>256</v>
       </c>
@@ -6302,7 +7693,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="61.9" customHeight="1">
-      <c r="A10" s="15"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>260</v>
       </c>
@@ -6318,7 +7709,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="60.6" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="18" t="s">
         <v>263</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -6338,7 +7729,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" customHeight="1">
-      <c r="A12" s="14"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>269</v>
       </c>
@@ -6356,7 +7747,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="51" customHeight="1">
-      <c r="A13" s="14"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="4" t="s">
         <v>273</v>
       </c>
@@ -6374,7 +7765,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="60.6" customHeight="1">
-      <c r="A14" s="14"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="4" t="s">
         <v>278</v>
       </c>
@@ -6392,7 +7783,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="62.45" customHeight="1">
-      <c r="A15" s="15"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="4" t="s">
         <v>283</v>
       </c>
@@ -6404,7 +7795,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="58.9" customHeight="1">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="18" t="s">
         <v>285</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -6424,7 +7815,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="58.15" customHeight="1">
-      <c r="A17" s="14"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>290</v>
       </c>
@@ -6442,7 +7833,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="59.45" customHeight="1">
-      <c r="A18" s="14"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>295</v>
       </c>
@@ -6460,7 +7851,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="60.6" customHeight="1">
-      <c r="A19" s="14"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
         <v>300</v>
       </c>
@@ -6478,7 +7869,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="60.6" customHeight="1">
-      <c r="A20" s="14"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="4" t="s">
         <v>305</v>
       </c>
@@ -6496,7 +7887,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="73.150000000000006" customHeight="1">
-      <c r="A21" s="15"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="4" t="s">
         <v>309</v>
       </c>
@@ -6510,7 +7901,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="61.15" customHeight="1">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="18" t="s">
         <v>311</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -6528,7 +7919,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="73.900000000000006" customHeight="1">
-      <c r="A23" s="14"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="4" t="s">
         <v>316</v>
       </c>
@@ -6546,7 +7937,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="67.150000000000006" customHeight="1">
-      <c r="A24" s="15"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="4" t="s">
         <v>321</v>
       </c>
@@ -6562,7 +7953,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="57" customHeight="1">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="18" t="s">
         <v>325</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -6580,7 +7971,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="64.150000000000006" customHeight="1">
-      <c r="A26" s="14"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="4" t="s">
         <v>330</v>
       </c>
@@ -6592,7 +7983,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="70.150000000000006" customHeight="1">
-      <c r="A27" s="14"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="4" t="s">
         <v>332</v>
       </c>
@@ -6610,7 +8001,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="55.15" customHeight="1">
-      <c r="A28" s="14"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="4" t="s">
         <v>337</v>
       </c>
@@ -6622,7 +8013,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="54" customHeight="1">
-      <c r="A29" s="14"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="4" t="s">
         <v>339</v>
       </c>
@@ -6640,7 +8031,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="45.6" customHeight="1">
-      <c r="A30" s="14"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="4" t="s">
         <v>344</v>
       </c>
@@ -6654,7 +8045,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="53.45" customHeight="1">
-      <c r="A31" s="14"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="4" t="s">
         <v>347</v>
       </c>
@@ -6672,7 +8063,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="47.25">
-      <c r="A32" s="15"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="4" t="s">
         <v>352</v>
       </c>
@@ -6706,8 +8097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F41" sqref="A1:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6742,14 +8133,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="31.15" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="10" t="s">
         <v>364</v>
       </c>
@@ -6815,14 +8206,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="31.15" customHeight="1">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="31.5">
       <c r="A7" s="1" t="s">
@@ -6965,14 +8356,14 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.15" customHeight="1">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:7" ht="15.75">
       <c r="A15" s="1" t="s">
@@ -7075,14 +8466,14 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="31.15" customHeight="1">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" ht="31.5">
       <c r="A21" s="1" t="s">
@@ -7285,14 +8676,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="31.15" customHeight="1">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="19"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:6" ht="31.5">
       <c r="A32" s="1" t="s">
@@ -7395,14 +8786,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="31.15" customHeight="1">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="13" t="s">
         <v>545</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="19"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" ht="31.5">
       <c r="A38" s="1" t="s">
@@ -7507,12 +8898,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D3ACDDDBD8A5C4593575E3E01142631" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8a293e8abb7ffc5713dd741c8c3e116b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="236434ac-9621-4ff5-a838-39e894409630" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a19c1cdb56b8a595505defc37df7bfbc" ns2:_="">
     <xsd:import namespace="236434ac-9621-4ff5-a838-39e894409630"/>
@@ -7656,6 +9041,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69FCB49C-165E-42F4-A168-DED652EE564F}">
   <ds:schemaRefs>
@@ -7665,15 +9056,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50986609-E751-43AA-B356-DAA8C5B3E7BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FBA87BA-F043-4DD6-BEC5-3BFA656C94EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7689,4 +9071,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50986609-E751-43AA-B356-DAA8C5B3E7BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>